<commit_message>
Lagd til demo på Henting av database til Statistikk og til excel fil. Nedlastbar excel fil
</commit_message>
<xml_diff>
--- a/EasyTimeWebApp/demo.xlsx
+++ b/EasyTimeWebApp/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Tid</t>
   </si>
@@ -23,15 +23,6 @@
   </si>
   <si>
     <t>Dato</t>
-  </si>
-  <si>
-    <t>12:30</t>
-  </si>
-  <si>
-    <t>Marius Sørenes</t>
-  </si>
-  <si>
-    <t>27.07.2016</t>
   </si>
 </sst>
 </file>
@@ -408,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,17 +421,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>